<commit_message>
fix: improve Project Euler 2 with a solution using array formulas + miscellaneous
</commit_message>
<xml_diff>
--- a/Project Euler 001.xlsx
+++ b/Project Euler 001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BB1392-1062-47ED-BAA1-F1C53DFCE854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1219E6-9894-4D3F-AB6E-52C75D53EB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D3559FC-258C-4822-AA11-34D88958350F}"/>
   </bookViews>
@@ -157,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -170,6 +170,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +508,7 @@
   <dimension ref="B2:K1011"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -551,42 +552,42 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" cm="1">
-        <f t="array" ref="B7" xml:space="preserve"> SUM(
-      _xlfn.MAP(
-            _xlfn.SEQUENCE(B6),
-            _xlfn.LAMBDA(_xlpm.N, IF(OR( MOD(_xlpm.N,3)=0, MOD(_xlpm.N,5)=0 ), _xlpm.N, 0))))</f>
+      <c r="B7" s="10" cm="1">
+        <f t="array" ref="B7">_xlfn.LET(
+_xlpm.MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N,OR(MOD(_xlpm.N,3)=0,MOD(_xlpm.N,5)=0)),
+_xlpm.FILTER_MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N, IF(_xlpm.MULTIPLE_OF_3_OR_5(_xlpm.N), _xlpm.N, 0)),
+SUM( _xlfn.MAP( _xlfn.SEQUENCE(B6), _xlpm.FILTER_MULTIPLE_OF_3_OR_5)))</f>
         <v>23</v>
       </c>
       <c r="D7" s="3" cm="1">
-        <f t="array" ref="D7" xml:space="preserve"> SUM(
-      _xlfn.MAP(
-            _xlfn.SEQUENCE(D6),
-            _xlfn.LAMBDA(_xlpm.N, IF(OR( MOD(_xlpm.N,3)=0, MOD(_xlpm.N,5)=0 ), _xlpm.N, 0))))</f>
+        <f t="array" ref="D7">_xlfn.LET(
+_xlpm.MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N,OR(MOD(_xlpm.N,3)=0,MOD(_xlpm.N,5)=0)),
+_xlpm.FILTER_MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N, IF(_xlpm.MULTIPLE_OF_3_OR_5(_xlpm.N), _xlpm.N, 0)),
+SUM( _xlfn.MAP( _xlfn.SEQUENCE(D6), _xlpm.FILTER_MULTIPLE_OF_3_OR_5)))</f>
         <v>233168</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="3" cm="1">
-        <f t="array" ref="G7" xml:space="preserve"> SUM(
-      _xlfn.MAP(
-            _xlfn.SEQUENCE(G6),
-            _xlfn.LAMBDA(_xlpm.N, IF(OR( MOD(_xlpm.N,3)=0, MOD(_xlpm.N,5)=0 ), _xlpm.N, 0))))</f>
+      <c r="G7" s="10" cm="1">
+        <f t="array" ref="G7">_xlfn.LET(
+_xlpm.MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N,OR(MOD(_xlpm.N,3)=0,MOD(_xlpm.N,5)=0)),
+_xlpm.FILTER_MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N, IF(_xlpm.MULTIPLE_OF_3_OR_5(_xlpm.N), _xlpm.N, 0)),
+SUM( _xlfn.MAP( _xlfn.SEQUENCE(G6), _xlpm.FILTER_MULTIPLE_OF_3_OR_5)))</f>
         <v>23331668</v>
       </c>
-      <c r="I7" s="3" cm="1">
-        <f t="array" ref="I7" xml:space="preserve"> SUM(
-      _xlfn.MAP(
-            _xlfn.SEQUENCE(I6),
-            _xlfn.LAMBDA(_xlpm.N, IF(OR( MOD(_xlpm.N,3)=0, MOD(_xlpm.N,5)=0 ), _xlpm.N, 0))))</f>
+      <c r="I7" s="10" cm="1">
+        <f t="array" ref="I7">_xlfn.LET(
+_xlpm.MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N,OR(MOD(_xlpm.N,3)=0,MOD(_xlpm.N,5)=0)),
+_xlpm.FILTER_MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N, IF(_xlpm.MULTIPLE_OF_3_OR_5(_xlpm.N), _xlpm.N, 0)),
+SUM( _xlfn.MAP( _xlfn.SEQUENCE(I6), _xlpm.FILTER_MULTIPLE_OF_3_OR_5)))</f>
         <v>2333316668</v>
       </c>
-      <c r="K7" s="3" cm="1">
-        <f t="array" ref="K7" xml:space="preserve"> SUM(
-      _xlfn.MAP(
-            _xlfn.SEQUENCE(K6),
-            _xlfn.LAMBDA(_xlpm.N, IF(OR( MOD(_xlpm.N,3)=0, MOD(_xlpm.N,5)=0 ), _xlpm.N, 0))))</f>
+      <c r="K7" s="10" cm="1">
+        <f t="array" ref="K7">_xlfn.LET(
+_xlpm.MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N,OR(MOD(_xlpm.N,3)=0,MOD(_xlpm.N,5)=0)),
+_xlpm.FILTER_MULTIPLE_OF_3_OR_5, _xlfn.LAMBDA(_xlpm.N, IF(_xlpm.MULTIPLE_OF_3_OR_5(_xlpm.N), _xlpm.N, 0)),
+SUM( _xlfn.MAP( _xlfn.SEQUENCE(K6), _xlpm.FILTER_MULTIPLE_OF_3_OR_5)))</f>
         <v>233333166668</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add explanations to 'Project Euler 5' section of README
</commit_message>
<xml_diff>
--- a/Project Euler 001.xlsx
+++ b/Project Euler 001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0D8C98-95E3-4440-A490-549C0B5ECE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6639C3B2-9023-402C-B6B8-89B0450D8722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D3559FC-258C-4822-AA11-34D88958350F}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="B2:K1026"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
feat: improve presentation details
</commit_message>
<xml_diff>
--- a/Project Euler 001.xlsx
+++ b/Project Euler 001.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noccis\Dropbox\1-projets\excel-problem-solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6639C3B2-9023-402C-B6B8-89B0450D8722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1F7071-273E-4A00-B451-84100384DCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D3559FC-258C-4822-AA11-34D88958350F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>&lt;-- answer</t>
   </si>
@@ -66,19 +66,7 @@
     <t>Numbers of the previous column if multiple of 3 or 5; otherwise 0</t>
   </si>
   <si>
-    <t>Projet Euler 1: Multiples of 3 or 5</t>
-  </si>
-  <si>
     <t>Successive integers below 1000</t>
-  </si>
-  <si>
-    <t>1) Recursion</t>
-  </si>
-  <si>
-    <t>4) Using spreadsheets capabilities</t>
-  </si>
-  <si>
-    <t>2) Tail-call recursion</t>
   </si>
   <si>
     <t>If we list all the natural numbers below 10 that are multiples of 3 or 5, we get 3, 5, 6 and 9.</t>
@@ -90,10 +78,25 @@
     <t>Find the sum of all the multiples of 3 or 5 below 1000.</t>
   </si>
   <si>
-    <t>3) As one-liner with array formulas</t>
+    <t>https://projecteuler.net/problem=1</t>
   </si>
   <si>
-    <t>https://projecteuler.net/problem=1</t>
+    <t>1) One-liner based on recursion</t>
+  </si>
+  <si>
+    <t>2) One-liner based on tail-call recursion</t>
+  </si>
+  <si>
+    <t>3) One-liner based on array formulas</t>
+  </si>
+  <si>
+    <t>4) Use of spreadsheets capabilities</t>
+  </si>
+  <si>
+    <t>Project Euler 1: Multiples of 3 or 5</t>
+  </si>
+  <si>
+    <t>(end)</t>
   </si>
 </sst>
 </file>
@@ -559,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB66A60-BC07-4716-90CD-37D3654E5F80}">
-  <dimension ref="B2:K1026"/>
+  <dimension ref="B2:K1028"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,7 +577,7 @@
   <sheetData>
     <row r="2" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -582,22 +585,22 @@
     </row>
     <row r="4" spans="2:11" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:11" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -605,7 +608,7 @@
     </row>
     <row r="9" spans="2:11" ht="16" x14ac:dyDescent="0.4">
       <c r="B9" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
@@ -673,7 +676,7 @@
     </row>
     <row r="14" spans="2:11" ht="16" x14ac:dyDescent="0.4">
       <c r="B14" s="10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
@@ -741,7 +744,7 @@
     </row>
     <row r="19" spans="2:11" ht="16" x14ac:dyDescent="0.4">
       <c r="B19" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
@@ -806,7 +809,7 @@
     </row>
     <row r="24" spans="2:11" ht="16" x14ac:dyDescent="0.4">
       <c r="B24" s="10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
@@ -828,7 +831,7 @@
     </row>
     <row r="28" spans="2:11" ht="116" x14ac:dyDescent="0.35">
       <c r="C28" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>1</v>
@@ -9798,7 +9801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1025" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="1025" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C1025" s="6">
         <v>998</v>
       </c>
@@ -9807,13 +9810,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1026" spans="3:4" x14ac:dyDescent="0.35">
+    <row r="1026" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C1026" s="6">
         <v>999</v>
       </c>
       <c r="D1026" s="6">
         <f t="shared" si="15"/>
         <v>999</v>
+      </c>
+    </row>
+    <row r="1028" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B1028" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>